<commit_message>
train the xlsx input. add gitignore
</commit_message>
<xml_diff>
--- a/randomData.xlsx
+++ b/randomData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuck\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\chuck21619\personal-projects\AI-practice\linear-regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3811688-D4BB-4D1A-B349-5D05D9203BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EA46D0-6088-452A-BD50-BB6288616D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6672" yWindow="960" windowWidth="30960" windowHeight="12204" xr2:uid="{C3CE96E3-909D-4FEA-B355-ADF8CACE5D84}"/>
+    <workbookView xWindow="60300" yWindow="5928" windowWidth="3324" windowHeight="6036" xr2:uid="{C3CE96E3-909D-4FEA-B355-ADF8CACE5D84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>house size</t>
+  </si>
+  <si>
+    <t>house price</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,84 +382,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F957C21-FD10-403E-A5D7-F5A271E4E68C}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>